<commit_message>
S3 Storage classes added
</commit_message>
<xml_diff>
--- a/S3/S3 Storage Classes.xlsx
+++ b/S3/S3 Storage Classes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaurav/Documents/UpGrad/AWS_Exam_Prep/AWSNotes/S3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2B22707-4E49-2248-8870-20C5C070B00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA15A16-2D82-9146-AD9B-0FF4BCBC504D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16000" xr2:uid="{81E098CC-CE01-6E42-B75B-43EE6C19AA94}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="1" xr2:uid="{81E098CC-CE01-6E42-B75B-43EE6C19AA94}"/>
   </bookViews>
   <sheets>
-    <sheet name="S3 Storage" sheetId="1" r:id="rId1"/>
+    <sheet name="S3 Storage Classes" sheetId="1" r:id="rId1"/>
+    <sheet name="S3 Pricing" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
   <si>
     <t>Standard</t>
   </si>
@@ -116,6 +117,83 @@
   </si>
   <si>
     <t>per GB retrieved</t>
+  </si>
+  <si>
+    <t>Storage Cost (per GB per month)</t>
+  </si>
+  <si>
+    <t>Retrieval Cost (per 100 requests)</t>
+  </si>
+  <si>
+    <t>Retrieval Time</t>
+  </si>
+  <si>
+    <t>Monitoring Cost (per 1000 objects)</t>
+  </si>
+  <si>
+    <t>$0.023</t>
+  </si>
+  <si>
+    <t>$0.0025 - $0.023</t>
+  </si>
+  <si>
+    <t>$0.0125</t>
+  </si>
+  <si>
+    <t>$0.01</t>
+  </si>
+  <si>
+    <t>$0.004</t>
+  </si>
+  <si>
+    <t>$0.0036</t>
+  </si>
+  <si>
+    <t>$0.00099</t>
+  </si>
+  <si>
+    <t>GET: $0.0004
+POST: $0.005</t>
+  </si>
+  <si>
+    <t>GET: $0.001
+POST: $0.01</t>
+  </si>
+  <si>
+    <t>GET: $0.001
+POST:$0.01</t>
+  </si>
+  <si>
+    <t>GET:$0.01
+POST:$0.02</t>
+  </si>
+  <si>
+    <t>GET: $0.0004
+POST:$0.03
+Expedited: $10
+Standard:$0.05
+Bulk:Free</t>
+  </si>
+  <si>
+    <t>GET:$0.0004
+POST:$0.05
+Standard:$0.10
+Bulk:$0.025</t>
+  </si>
+  <si>
+    <t>Instantaneous</t>
+  </si>
+  <si>
+    <t>Expedited: 1 -5 mins
+Standard: 3 - 5 hours
+Bulk: 5- 10 hours</t>
+  </si>
+  <si>
+    <t>Standard: 12 hours
+Bulk: 48 hours</t>
+  </si>
+  <si>
+    <t>$0.025</t>
   </si>
 </sst>
 </file>
@@ -162,7 +240,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -185,11 +263,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -205,6 +320,15 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,7 +646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AB8156-4DFB-EF40-AD49-C2ECD4D211C5}">
   <dimension ref="B4:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -757,4 +881,168 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927197A6-B66F-774C-8E04-1440B040D34B}">
+  <dimension ref="B4:J10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="29.83203125" customWidth="1"/>
+    <col min="8" max="8" width="29.33203125" customWidth="1"/>
+    <col min="9" max="9" width="33.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:10" ht="22" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="2:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="2:10" ht="44" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="2:10" ht="132" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="2:10" ht="66" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="2:10" ht="44" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C8:G8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>